<commit_message>
allow ref genome defined in index file
</commit_message>
<xml_diff>
--- a/sampleData/indexFiles/publicDataIndex.xlsx
+++ b/sampleData/indexFiles/publicDataIndex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MATLAB\gsfat\sampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MATLAB\4DNvestigator\sampleData\indexFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{254E8F58-0C2F-4A2F-B58B-885358A98B6F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F965CB32-931A-4856-9DB6-9B3B002DB1C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="15225" xr2:uid="{462294A1-CA47-4640-BA68-1B0CCE6FCF16}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>path</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>HUVEC</t>
+  </si>
+  <si>
+    <t>refGenome</t>
+  </si>
+  <si>
+    <t>hg19</t>
+  </si>
+  <si>
+    <t>HFFc6</t>
+  </si>
+  <si>
+    <t>H1-hESC</t>
+  </si>
+  <si>
+    <t>HFF-hTERT</t>
+  </si>
+  <si>
+    <t>hg38</t>
+  </si>
+  <si>
+    <t>https://data.4dnucleome.org/files-processed/4DNFIFLJLIS5/@@download/4DNFIFLJLIS5.hic</t>
+  </si>
+  <si>
+    <t>https://data.4dnucleome.org/files-processed/4DNFIOX3BGNE/@@download/4DNFIOX3BGNE.hic</t>
+  </si>
+  <si>
+    <t>https://data.4dnucleome.org/files-processed/4DNFIZ4F74QR/@@download/4DNFIZ4F74QR.hic</t>
   </si>
 </sst>
 </file>
@@ -429,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027636B9-280B-4387-B381-13FDFAF63BD4}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +469,7 @@
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +482,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -469,8 +499,11 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -483,8 +516,11 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -497,8 +533,11 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -511,8 +550,11 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -525,8 +567,11 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -539,56 +584,92 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>